<commit_message>
Fixed to support files from sverre
</commit_message>
<xml_diff>
--- a/CSV/DEMAND_DATAFRAME_SVERRE.xlsx
+++ b/CSV/DEMAND_DATAFRAME_SVERRE.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f9d71f9bda8fdeb6/Dokumenter/NTNU notater/10.semester/Masteroppgave^J Sigurd og Lars/structuralCircle/CSV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu.sharepoint.com/sites/o365_Artur-PhD/Shared Documents/General/Presentations and publications/2022.xx Oslo reuse project, mapping algorithm/Paper development/Data from IFC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_60A134875B905B07FF5B3311595ED87656CD5FFD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E9FA12F-B508-4F82-9E08-8A7C00DC2581}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{372C1109-9CC7-42D9-A809-A2D5D131FDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D749F918-D003-4D27-8D3B-3F236A1799C5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="49">
   <si>
     <t>Guid</t>
   </si>
@@ -133,6 +146,18 @@
     <t>2Ei2TUNq5A5uP_5j7Za17P</t>
   </si>
   <si>
+    <t>3v3NVdB_5AN9wXWv14hbye</t>
+  </si>
+  <si>
+    <t>3v3NVdB_5AN9wXWv14hb$B</t>
+  </si>
+  <si>
+    <t>3v3NVdB_5AN9wXWv14hb$k</t>
+  </si>
+  <si>
+    <t>3v3NVdB_5AN9wXWv14hb$m</t>
+  </si>
+  <si>
     <t>3fv9Tll3nCJw5Izn0UdNXG</t>
   </si>
   <si>
@@ -149,6 +174,9 @@
   </si>
   <si>
     <t>3fv9Tll3nCJw5Izn0UdNB1</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
   <si>
     <t>Moment of Inertia [m^4]</t>
@@ -158,7 +186,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +198,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -207,16 +241,85 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -229,8 +332,24 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F91C3C2A-2FFA-4CFA-9D88-BBC35C3B015B}" name="Table1" displayName="Table1" ref="A1:I39" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:I39" xr:uid="{F91C3C2A-2FFA-4CFA-9D88-BBC35C3B015B}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{33255180-0C92-4881-A0CC-00534D637D4F}" name="Column1" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{7E6D71AE-F787-4CA2-9D49-D10ADD77C1C5}" name="Guid"/>
+    <tableColumn id="3" xr3:uid="{431204F6-4E40-46DE-9886-FDA65DBB9CE4}" name="Length [m]"/>
+    <tableColumn id="4" xr3:uid="{179EF25C-F63F-41C0-8979-E701CE33FFE4}" name="Area [m^2]"/>
+    <tableColumn id="5" xr3:uid="{840D1D82-9F23-4F22-80F5-A70262699B76}" name="Moment of Inertia [m^4]" dataDxfId="0">
+      <calculatedColumnFormula>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{76C4F9D9-7D74-460C-A3C8-63191A520055}" name="Material"/>
+    <tableColumn id="7" xr3:uid="{87A5F30D-726B-41E6-A422-50D1E705936D}" name="Location"/>
+    <tableColumn id="8" xr3:uid="{9EAC117C-CD9F-465E-90A0-6A55F28FCF5E}" name="Latitude"/>
+    <tableColumn id="9" xr3:uid="{104449E2-7462-4963-8148-1C2E25DF455A}" name="Longitude"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -518,23 +637,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,8 +668,8 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>43</v>
+      <c r="E1" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -560,7 +684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -571,7 +695,11 @@
         <v>7.7205999999999992</v>
       </c>
       <c r="D2">
-        <v>9.6936369259886561</v>
+        <v>9.6936369259886593E-3</v>
+      </c>
+      <c r="E2">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>7.8305497377409058E-6</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -586,7 +714,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -597,7 +725,11 @@
         <v>7.7205999999999992</v>
       </c>
       <c r="D3">
-        <v>9.6936369259886561</v>
+        <v>9.6936369259886558E-3</v>
+      </c>
+      <c r="E3">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>7.830549737740899E-6</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -612,7 +744,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -623,7 +755,11 @@
         <v>7.7205999999999992</v>
       </c>
       <c r="D4">
-        <v>9.6936369259886934</v>
+        <v>9.693636925988694E-3</v>
+      </c>
+      <c r="E4">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>7.83054973774096E-6</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -638,7 +774,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -649,7 +785,11 @@
         <v>7.7205999999999966</v>
       </c>
       <c r="D5">
-        <v>9.1023109033614027</v>
+        <v>9.6936369260000495E-3</v>
+      </c>
+      <c r="E5">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>7.8305497377593067E-6</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
@@ -664,7 +804,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -675,7 +815,11 @@
         <v>7.7205999999999966</v>
       </c>
       <c r="D6">
-        <v>9.1023109033526044</v>
+        <v>9.6936369260000477E-3</v>
+      </c>
+      <c r="E6">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>7.8305497377593033E-6</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
@@ -690,7 +834,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -701,7 +845,11 @@
         <v>7.7205999999999966</v>
       </c>
       <c r="D7">
-        <v>9.1023109033525778</v>
+        <v>9.6936369260000529E-3</v>
+      </c>
+      <c r="E7">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>7.8305497377593135E-6</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -716,7 +864,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -727,7 +875,11 @@
         <v>7.7205999999999966</v>
       </c>
       <c r="D8">
-        <v>9.1023109033614915</v>
+        <v>9.6936369260000512E-3</v>
+      </c>
+      <c r="E8">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>7.8305497377593101E-6</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -742,7 +894,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -753,7 +905,11 @@
         <v>7.8097539999999972</v>
       </c>
       <c r="D9">
-        <v>9.8054607805513765</v>
+        <v>9.8054607805513772E-3</v>
+      </c>
+      <c r="E9">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.0122550932442682E-6</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -768,7 +924,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -779,7 +935,11 @@
         <v>7.8097539999999963</v>
       </c>
       <c r="D10">
-        <v>9.8054607805513747</v>
+        <v>9.8054607805513755E-3</v>
+      </c>
+      <c r="E10">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.0122550932442648E-6</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
@@ -794,7 +954,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -805,7 +965,11 @@
         <v>7.8097539999999972</v>
       </c>
       <c r="D11">
-        <v>9.8054607805513765</v>
+        <v>9.8054607805513772E-3</v>
+      </c>
+      <c r="E11">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.0122550932442682E-6</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -820,7 +984,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -831,7 +995,11 @@
         <v>7.8097539999999963</v>
       </c>
       <c r="D12">
-        <v>9.8054607805513747</v>
+        <v>9.8054607805513755E-3</v>
+      </c>
+      <c r="E12">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.0122550932442648E-6</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
@@ -846,7 +1014,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -857,7 +1025,11 @@
         <v>7.7205999999999992</v>
       </c>
       <c r="D13">
-        <v>9.6936369259886757</v>
+        <v>9.6936369259886766E-3</v>
+      </c>
+      <c r="E13">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>7.8305497377409329E-6</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -872,7 +1044,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -883,7 +1055,11 @@
         <v>7.9999999999999956</v>
       </c>
       <c r="D14">
-        <v>10.044082054247941</v>
+        <v>1.0044082054247941E-2</v>
+      </c>
+      <c r="E14">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.4069653593721274E-6</v>
       </c>
       <c r="F14" t="s">
         <v>8</v>
@@ -898,7 +1074,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -909,7 +1085,11 @@
         <v>7.9999999999999956</v>
       </c>
       <c r="D15">
-        <v>10.04408205424795</v>
+        <v>1.0044082054247949E-2</v>
+      </c>
+      <c r="E15">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.4069653593721409E-6</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
@@ -924,7 +1104,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -935,7 +1115,11 @@
         <v>7.9999999999999956</v>
       </c>
       <c r="D16">
-        <v>10.044082054247941</v>
+        <v>1.0044082054247941E-2</v>
+      </c>
+      <c r="E16">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.4069653593721274E-6</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
@@ -950,7 +1134,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -961,7 +1145,11 @@
         <v>7.9999999999999938</v>
       </c>
       <c r="D17">
-        <v>10.0440820542479</v>
+        <v>1.0044082054247901E-2</v>
+      </c>
+      <c r="E17">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.4069653593720596E-6</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
@@ -976,7 +1164,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -987,7 +1175,11 @@
         <v>7.9999999999999947</v>
       </c>
       <c r="D18">
-        <v>10.044082054247941</v>
+        <v>1.0044082054247941E-2</v>
+      </c>
+      <c r="E18">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.4069653593721274E-6</v>
       </c>
       <c r="F18" t="s">
         <v>8</v>
@@ -1002,7 +1194,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1013,7 +1205,11 @@
         <v>7.9999999999999956</v>
       </c>
       <c r="D19">
-        <v>10.04408205424795</v>
+        <v>1.0044082054247949E-2</v>
+      </c>
+      <c r="E19">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.4069653593721409E-6</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
@@ -1028,7 +1224,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1039,7 +1235,11 @@
         <v>7.9999999999999947</v>
       </c>
       <c r="D20">
-        <v>10.044082054247941</v>
+        <v>1.0044082054247941E-2</v>
+      </c>
+      <c r="E20">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.4069653593721274E-6</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
@@ -1054,7 +1254,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1065,7 +1265,11 @@
         <v>7.9999999999999947</v>
       </c>
       <c r="D21">
-        <v>10.044082054247911</v>
+        <v>1.0044082054247911E-2</v>
+      </c>
+      <c r="E21">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.4069653593720782E-6</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
@@ -1080,7 +1284,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1091,7 +1295,11 @@
         <v>7.8097539999999981</v>
       </c>
       <c r="D22">
-        <v>9.8054607805511811</v>
+        <v>9.8054607805511812E-3</v>
+      </c>
+      <c r="E22">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.012255093243948E-6</v>
       </c>
       <c r="F22" t="s">
         <v>8</v>
@@ -1106,7 +1314,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1117,7 +1325,11 @@
         <v>7.8097539999999972</v>
       </c>
       <c r="D23">
-        <v>9.8054607805514085</v>
+        <v>9.8054607805514084E-3</v>
+      </c>
+      <c r="E23">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.012255093244319E-6</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
@@ -1132,7 +1344,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1143,7 +1355,11 @@
         <v>7.8097539999999981</v>
       </c>
       <c r="D24">
-        <v>9.8054607805514085</v>
+        <v>9.8054607805514084E-3</v>
+      </c>
+      <c r="E24">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.012255093244319E-6</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
@@ -1158,7 +1374,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1169,7 +1385,11 @@
         <v>7.8097539999999963</v>
       </c>
       <c r="D25">
-        <v>9.8054607805514085</v>
+        <v>9.8054607805514084E-3</v>
+      </c>
+      <c r="E25">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.012255093244319E-6</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
@@ -1184,7 +1404,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1195,7 +1415,11 @@
         <v>7.9999999999999956</v>
       </c>
       <c r="D26">
-        <v>10.04408205424795</v>
+        <v>1.0044082054247949E-2</v>
+      </c>
+      <c r="E26">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.4069653593721409E-6</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
@@ -1210,7 +1434,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1221,7 +1445,11 @@
         <v>7.9999999999999973</v>
       </c>
       <c r="D27">
-        <v>10.0440820542479</v>
+        <v>1.0044082054247901E-2</v>
+      </c>
+      <c r="E27">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.4069653593720596E-6</v>
       </c>
       <c r="F27" t="s">
         <v>8</v>
@@ -1236,7 +1464,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1247,7 +1475,11 @@
         <v>7.9999999999999956</v>
       </c>
       <c r="D28">
-        <v>10.04408205424795</v>
+        <v>1.0044082054247949E-2</v>
+      </c>
+      <c r="E28">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.4069653593721409E-6</v>
       </c>
       <c r="F28" t="s">
         <v>8</v>
@@ -1262,7 +1494,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1273,7 +1505,11 @@
         <v>7.9999999999999956</v>
       </c>
       <c r="D29">
-        <v>10.0440820542479</v>
+        <v>1.0044082054247901E-2</v>
+      </c>
+      <c r="E29">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.4069653593720596E-6</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
@@ -1288,7 +1524,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1296,10 +1532,14 @@
         <v>37</v>
       </c>
       <c r="C30">
-        <v>3.1</v>
+        <v>7.9796453762421917</v>
       </c>
       <c r="D30">
-        <v>4.6213798266582264</v>
+        <v>1.001855170802937E-2</v>
+      </c>
+      <c r="E30">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.36428152720485E-6</v>
       </c>
       <c r="F30" t="s">
         <v>8</v>
@@ -1314,7 +1554,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1322,10 +1562,14 @@
         <v>38</v>
       </c>
       <c r="C31">
-        <v>5.5</v>
+        <v>7.9796453762421979</v>
       </c>
       <c r="D31">
-        <v>8.1847969516294388</v>
+        <v>1.0018551708029391E-2</v>
+      </c>
+      <c r="E31">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.3642815272048855E-6</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
@@ -1340,7 +1584,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1348,10 +1592,14 @@
         <v>39</v>
       </c>
       <c r="C32">
-        <v>3.1</v>
+        <v>7.9796453762421979</v>
       </c>
       <c r="D32">
-        <v>4.6213798266582264</v>
+        <v>1.0018551708029341E-2</v>
+      </c>
+      <c r="E32">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.3642815272048008E-6</v>
       </c>
       <c r="F32" t="s">
         <v>8</v>
@@ -1366,7 +1614,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1374,10 +1622,14 @@
         <v>40</v>
       </c>
       <c r="C33">
-        <v>3.1</v>
+        <v>7.9796453762421908</v>
       </c>
       <c r="D33">
-        <v>4.6213798266582264</v>
+        <v>1.001855170802936E-2</v>
+      </c>
+      <c r="E33">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>8.364281527204833E-6</v>
       </c>
       <c r="F33" t="s">
         <v>8</v>
@@ -1392,7 +1644,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1400,10 +1652,14 @@
         <v>41</v>
       </c>
       <c r="C34">
-        <v>5.5</v>
+        <v>3.1</v>
       </c>
       <c r="D34">
-        <v>8.1847969516294388</v>
+        <v>4.6213798266582264E-3</v>
+      </c>
+      <c r="E34">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>1.7797626251869681E-6</v>
       </c>
       <c r="F34" t="s">
         <v>8</v>
@@ -1418,7 +1674,7 @@
         <v>10.729945182777779</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1426,25 +1682,153 @@
         <v>42</v>
       </c>
       <c r="C35">
+        <v>5.5</v>
+      </c>
+      <c r="D35">
+        <v>8.1847969516294396E-3</v>
+      </c>
+      <c r="E35">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>5.5825750949502136E-6</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35">
+        <v>59.941616058333331</v>
+      </c>
+      <c r="I35">
+        <v>10.729945182777779</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36">
         <v>3.1</v>
       </c>
-      <c r="D35">
-        <v>4.6213798266582264</v>
-      </c>
-      <c r="F35" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" t="s">
-        <v>9</v>
-      </c>
-      <c r="H35">
-        <v>59.941616058333331</v>
-      </c>
-      <c r="I35">
+      <c r="D36">
+        <v>4.6213798266582264E-3</v>
+      </c>
+      <c r="E36">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>1.7797626251869681E-6</v>
+      </c>
+      <c r="F36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36">
+        <v>59.941616058333331</v>
+      </c>
+      <c r="I36">
+        <v>10.729945182777779</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37">
+        <v>3.1</v>
+      </c>
+      <c r="D37">
+        <v>4.6213798266582264E-3</v>
+      </c>
+      <c r="E37">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>1.7797626251869681E-6</v>
+      </c>
+      <c r="F37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37">
+        <v>59.941616058333331</v>
+      </c>
+      <c r="I37">
+        <v>10.729945182777779</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38">
+        <v>5.5</v>
+      </c>
+      <c r="D38">
+        <v>8.1847969516294396E-3</v>
+      </c>
+      <c r="E38">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>5.5825750949502136E-6</v>
+      </c>
+      <c r="F38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38">
+        <v>59.941616058333331</v>
+      </c>
+      <c r="I38">
+        <v>10.729945182777779</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39">
+        <v>3.1</v>
+      </c>
+      <c r="D39">
+        <v>4.6213798266582264E-3</v>
+      </c>
+      <c r="E39">
+        <f>1/12 *Table1[[#This Row],[Area '[m^2']]]^2</f>
+        <v>1.7797626251869681E-6</v>
+      </c>
+      <c r="F39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39">
+        <v>59.941616058333331</v>
+      </c>
+      <c r="I39">
         <v>10.729945182777779</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>